<commit_message>
Coinbase API access secured
</commit_message>
<xml_diff>
--- a/Exchange Trading Scripts/Exchange API Access Tracker.xlsx
+++ b/Exchange Trading Scripts/Exchange API Access Tracker.xlsx
@@ -138,7 +138,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -153,16 +153,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -445,7 +435,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -530,7 +520,7 @@
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2">
         <v>25000</v>
@@ -722,13 +712,13 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Updated tracker....Several exchanges are closed for new customers
</commit_message>
<xml_diff>
--- a/Exchange Trading Scripts/Exchange API Access Tracker.xlsx
+++ b/Exchange Trading Scripts/Exchange API Access Tracker.xlsx
@@ -18,6 +18,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{0D27129A-8733-40CB-882E-68AAA4E9E130}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cannot Set Up New Accounts</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
   <si>
@@ -100,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,13 +142,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,11 +188,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,11 +492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -597,7 +658,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1">
@@ -629,7 +690,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1">
@@ -661,7 +722,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="1">
@@ -725,7 +786,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="1">
@@ -738,7 +799,7 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -774,5 +835,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>